<commit_message>
Resolved issues related to system Setup
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/CRUD-Organizational Dept.xlsx
+++ b/templates/AutomationOrg/CRUD-Organizational Dept.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkakade\Provar\Workspace\System Setup\templates\AutomationOrg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\provar\QA-automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FCEF1D-41E4-4C86-B76B-8747B68294FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A754CA-61F1-4B0D-A666-F2BF87F39EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36" yWindow="1632" windowWidth="15912" windowHeight="8964" xr2:uid="{DF5D691F-F604-4F70-890B-2E03CF1489E1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DF5D691F-F604-4F70-890B-2E03CF1489E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Create_Org" sheetId="2" r:id="rId1"/>
@@ -430,12 +430,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D53189-0C97-4159-AF7E-3B1A48C92BE7}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -475,9 +481,6 @@
       </c>
       <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -498,13 +501,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBC8DDF-D394-41E1-A31F-1ABB9B51A0DF}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -544,11 +553,8 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>

</xml_diff>